<commit_message>
Added BuyerName to spreadsheet
</commit_message>
<xml_diff>
--- a/AmbRcnTradeServer/ExcelTemplates/InspectionExportTemplate.xlsx
+++ b/AmbRcnTradeServer/ExcelTemplates/InspectionExportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Studio\AmbRcnTrade\AmbRcnTradeServer\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A65340C-052A-45EE-AA67-8420DE705903}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BD30DD-B565-4C69-98C1-53C662F08572}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="10680" windowWidth="38640" windowHeight="21240" xr2:uid="{6E18A325-C572-4F19-8B68-4B2A3EEFB2AD}"/>
   </bookViews>
@@ -16,21 +16,21 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$O$7</definedName>
-    <definedName name="Avg_bag_weight">Sheet1!$K$8:$K$1048576</definedName>
-    <definedName name="Bags">Sheet1!$H$8:$H$1048576</definedName>
-    <definedName name="Count">Sheet1!$M$8:$M$1048576</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$P$7</definedName>
+    <definedName name="Avg_bag_weight">Sheet1!$L$8:$L$1048576</definedName>
+    <definedName name="Bags">Sheet1!$I$8:$I$1048576</definedName>
+    <definedName name="Count">Sheet1!$N$8:$N$1048576</definedName>
     <definedName name="Date">Sheet1!$B$8:$B$1048576</definedName>
-    <definedName name="Fiche">Sheet1!$E$8:$E$1048576</definedName>
+    <definedName name="Fiche">Sheet1!$F$8:$F$1048576</definedName>
     <definedName name="Inspection">Sheet1!$A$8:$A$1048576</definedName>
-    <definedName name="Kg">Sheet1!$I$8:$I$1048576</definedName>
-    <definedName name="KOR">Sheet1!$L$8:$L$1048576</definedName>
-    <definedName name="Moisture">Sheet1!$N$8:$N$1048576</definedName>
-    <definedName name="Price">Sheet1!$G$8:$G$1048576</definedName>
-    <definedName name="Rejects">Sheet1!$O$8:$O$1048576</definedName>
-    <definedName name="Supplier">Sheet1!$D$8:$D$1048576</definedName>
-    <definedName name="Truck">Sheet1!$F$8:$F$1048576</definedName>
-    <definedName name="Value_CFA">Sheet1!$J$8:$J$1048576</definedName>
+    <definedName name="Kg">Sheet1!$J$8:$J$1048576</definedName>
+    <definedName name="KOR">Sheet1!$M$8:$M$1048576</definedName>
+    <definedName name="Moisture">Sheet1!$O$8:$O$1048576</definedName>
+    <definedName name="Price">Sheet1!$H$8:$H$1048576</definedName>
+    <definedName name="Rejects">Sheet1!$P$8:$P$1048576</definedName>
+    <definedName name="Supplier">Sheet1!$E$8:$E$1048576</definedName>
+    <definedName name="Truck">Sheet1!$G$8:$G$1048576</definedName>
+    <definedName name="Value_CFA">Sheet1!$K$8:$K$1048576</definedName>
     <definedName name="Warehouse">Sheet1!$C$8:$C$1048576</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Inspection</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Average moisture</t>
+  </si>
+  <si>
+    <t>Buyer</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -271,14 +274,14 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -601,30 +604,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC63CF19-5699-4FF3-9B6E-8DCAA97A77B2}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:O7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.453125" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" customWidth="1"/>
-    <col min="6" max="6" width="25.90625" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.6328125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.54296875" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="18"/>
-    <col min="15" max="15" width="8.7265625" style="4"/>
-    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.90625" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.6328125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="18"/>
+    <col min="16" max="16" width="8.7265625" style="4"/>
+    <col min="18" max="18" width="16.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -633,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
@@ -642,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
@@ -651,7 +654,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
@@ -660,7 +663,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
         <v>19</v>
       </c>
@@ -669,7 +672,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,57 +683,60 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="J8" s="10">
-        <f>I8*G8</f>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K8" s="10">
+        <f>J8*H8</f>
         <v>0</v>
       </c>
-      <c r="K8" s="3" t="e">
-        <f>I8/H8</f>
+      <c r="L8" s="3" t="e">
+        <f>J8/I8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>45.7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:O7" xr:uid="{8CE4A24E-279B-40EF-B2E9-FE5060022E31}"/>
+  <autoFilter ref="A7:P7" xr:uid="{8CE4A24E-279B-40EF-B2E9-FE5060022E31}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>